<commit_message>
ongoing testing work ... ongoing work on MockClientMiddleware tests.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/MockClient/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/MockClient/TestJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\MockClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBB0FFC-824E-4D24-8F6F-E6254F4C3BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74430C-0C39-44D3-A377-6A7139C0FB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="248" yWindow="593" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="248" yWindow="0" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
   <si>
     <t>ProjectName</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>GetB</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -448,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -457,8 +469,8 @@
     <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1328125" style="1"/>
@@ -497,8 +509,11 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -517,8 +532,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -537,8 +555,11 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
@@ -557,8 +578,11 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -577,8 +601,11 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>12</v>
@@ -597,8 +624,11 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
@@ -617,8 +647,11 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
@@ -637,8 +670,11 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
@@ -657,8 +693,11 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
@@ -677,8 +716,11 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -697,8 +739,11 @@
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>12</v>
@@ -717,8 +762,11 @@
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>7</v>
@@ -737,8 +785,11 @@
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>12</v>
@@ -757,8 +808,11 @@
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -777,8 +831,11 @@
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>12</v>
@@ -797,8 +854,11 @@
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
MockClientMiddleware tests now working.  Also, refactored test APIs to use distinct ports.
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/MockClient/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/MockClient/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\MockClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\MockClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74430C-0C39-44D3-A377-6A7139C0FB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E68E9C-D350-4046-9DFF-D6CCA9832FB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="248" yWindow="0" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="25080" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,22 +461,22 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -522,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -545,7 +545,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -568,7 +568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -591,7 +591,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -637,7 +637,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -660,7 +660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -680,10 +680,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="1">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -706,7 +706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -729,7 +729,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -752,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -775,7 +775,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -798,7 +798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -818,10 +818,10 @@
         <v>7</v>
       </c>
       <c r="G15" s="1">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,7 +844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>